<commit_message>
update de estructura y correccion de bugs
</commit_message>
<xml_diff>
--- a/DATA/distance_tables.xlsx
+++ b/DATA/distance_tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franklin\Documents\Schollarships\APORTA\Challenge_Sinfonia\SINFONIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEA74EB-FF91-4AA7-9D8E-F66AA765CBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB82F6C3-AE19-4C7B-B285-D4C25151D19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58CB8F78-7FE5-4B8A-9C47-6775F6B9FD5D}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="distance" sheetId="1" r:id="rId1"/>
     <sheet name="neighboor" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -144,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,12 +497,15 @@
   <dimension ref="A1:AJ36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AJ1"/>
+      <selection activeCell="AI34" sqref="AI34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +612,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -715,7 +722,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -821,8 +828,11 @@
       <c r="AI3">
         <v>11.9</v>
       </c>
+      <c r="AJ3">
+        <v>49.1</v>
+      </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -850,9 +860,21 @@
       <c r="I4">
         <v>2</v>
       </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
       <c r="K4">
         <v>5.5</v>
       </c>
+      <c r="L4">
+        <v>2.7</v>
+      </c>
+      <c r="M4">
+        <v>12.9</v>
+      </c>
+      <c r="N4">
+        <v>4.5999999999999996</v>
+      </c>
       <c r="O4">
         <v>4.9000000000000004</v>
       </c>
@@ -865,12 +887,18 @@
       <c r="R4">
         <v>9.3000000000000007</v>
       </c>
+      <c r="S4">
+        <v>9.9</v>
+      </c>
       <c r="T4">
         <v>5.8</v>
       </c>
       <c r="U4">
         <v>6</v>
       </c>
+      <c r="V4">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="W4">
         <v>8.4</v>
       </c>
@@ -880,6 +908,9 @@
       <c r="Y4">
         <v>14.4</v>
       </c>
+      <c r="Z4">
+        <v>22.9</v>
+      </c>
       <c r="AA4">
         <v>19.3</v>
       </c>
@@ -907,8 +938,11 @@
       <c r="AI4">
         <v>9.4</v>
       </c>
+      <c r="AJ4">
+        <v>39.6</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -925,7 +959,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="G5">
         <v>1.7</v>
@@ -954,6 +988,9 @@
       <c r="O5">
         <v>4.0999999999999996</v>
       </c>
+      <c r="P5">
+        <v>9.1</v>
+      </c>
       <c r="Q5">
         <v>4.9000000000000004</v>
       </c>
@@ -964,7 +1001,7 @@
         <v>5</v>
       </c>
       <c r="T5">
-        <v>8.1999999999999993</v>
+        <v>8.1</v>
       </c>
       <c r="U5">
         <v>7.7</v>
@@ -979,31 +1016,31 @@
         <v>15</v>
       </c>
       <c r="Y5">
-        <v>17</v>
+        <v>27.2</v>
       </c>
       <c r="Z5">
         <v>11</v>
       </c>
       <c r="AA5">
-        <v>21</v>
+        <v>28.6</v>
       </c>
       <c r="AB5">
         <v>22</v>
       </c>
       <c r="AC5">
-        <v>8</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="AD5">
-        <v>15</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="AE5">
-        <v>21</v>
+        <v>21.3</v>
       </c>
       <c r="AF5">
-        <v>11</v>
+        <v>11.2</v>
       </c>
       <c r="AG5">
-        <v>13</v>
+        <v>12.9</v>
       </c>
       <c r="AH5">
         <v>15.1</v>
@@ -1011,8 +1048,11 @@
       <c r="AI5">
         <v>10.8</v>
       </c>
+      <c r="AJ5">
+        <v>45.6</v>
+      </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1067,6 +1107,9 @@
       <c r="R6">
         <v>7.8</v>
       </c>
+      <c r="S6">
+        <v>20.2</v>
+      </c>
       <c r="T6">
         <v>8.6999999999999993</v>
       </c>
@@ -1076,6 +1119,9 @@
       <c r="V6">
         <v>10.5</v>
       </c>
+      <c r="W6">
+        <v>11.4</v>
+      </c>
       <c r="X6">
         <v>9.9</v>
       </c>
@@ -1089,16 +1135,16 @@
         <v>22</v>
       </c>
       <c r="AB6">
-        <v>21</v>
+        <v>21.4</v>
       </c>
       <c r="AC6">
-        <v>13</v>
+        <v>13.2</v>
       </c>
       <c r="AD6">
         <v>16</v>
       </c>
       <c r="AE6">
-        <v>20</v>
+        <v>19.5</v>
       </c>
       <c r="AF6">
         <v>13</v>
@@ -1116,7 +1162,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1222,8 +1268,11 @@
       <c r="AI7">
         <v>9.1999999999999993</v>
       </c>
+      <c r="AJ7">
+        <v>45.6</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1281,6 +1330,15 @@
       <c r="S8">
         <v>7.3</v>
       </c>
+      <c r="T8">
+        <v>27.7</v>
+      </c>
+      <c r="U8">
+        <v>22</v>
+      </c>
+      <c r="V8">
+        <v>3</v>
+      </c>
       <c r="W8">
         <v>6.8</v>
       </c>
@@ -1297,16 +1355,16 @@
         <v>24</v>
       </c>
       <c r="AB8">
-        <v>19</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="AC8">
-        <v>8</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="AD8">
         <v>18</v>
       </c>
       <c r="AE8">
-        <v>18</v>
+        <v>18.3</v>
       </c>
       <c r="AF8">
         <v>14</v>
@@ -1324,7 +1382,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1356,11 +1414,14 @@
         <v>3.4</v>
       </c>
       <c r="K9">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="L9">
         <v>4.3</v>
       </c>
+      <c r="M9">
+        <v>11.8</v>
+      </c>
       <c r="N9">
         <v>1.8</v>
       </c>
@@ -1389,10 +1450,10 @@
         <v>4.3</v>
       </c>
       <c r="W9">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="X9">
-        <v>14</v>
+        <v>13.8</v>
       </c>
       <c r="Y9">
         <v>13</v>
@@ -1401,25 +1462,25 @@
         <v>14</v>
       </c>
       <c r="AA9">
-        <v>18</v>
+        <v>17.7</v>
       </c>
       <c r="AB9">
-        <v>26</v>
+        <v>36.9</v>
       </c>
       <c r="AC9">
-        <v>11</v>
+        <v>11.1</v>
       </c>
       <c r="AD9">
-        <v>12</v>
+        <v>11.6</v>
       </c>
       <c r="AE9">
-        <v>25</v>
+        <v>29.5</v>
       </c>
       <c r="AF9">
         <v>7.5</v>
       </c>
       <c r="AG9">
-        <v>10</v>
+        <v>9.6</v>
       </c>
       <c r="AH9">
         <v>12.5</v>
@@ -1427,8 +1488,11 @@
       <c r="AI9">
         <v>7.4</v>
       </c>
+      <c r="AJ9">
+        <v>42</v>
+      </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1438,6 +1502,9 @@
       <c r="C10">
         <v>5.6</v>
       </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
       <c r="E10">
         <v>2.6</v>
       </c>
@@ -1457,7 +1524,16 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>9.1999999999999993</v>
+        <v>11</v>
+      </c>
+      <c r="L10">
+        <v>8.5</v>
+      </c>
+      <c r="M10">
+        <v>10.8</v>
+      </c>
+      <c r="N10">
+        <v>1.9</v>
       </c>
       <c r="O10">
         <v>1.6</v>
@@ -1471,15 +1547,33 @@
       <c r="R10">
         <v>9.6999999999999993</v>
       </c>
+      <c r="S10">
+        <v>3</v>
+      </c>
       <c r="T10">
         <v>7.6</v>
       </c>
       <c r="U10">
         <v>6.3</v>
       </c>
+      <c r="V10">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="W10">
         <v>5.2</v>
       </c>
+      <c r="X10">
+        <v>22.5</v>
+      </c>
+      <c r="Y10">
+        <v>22.5</v>
+      </c>
+      <c r="Z10">
+        <v>19.8</v>
+      </c>
+      <c r="AA10">
+        <v>23.7</v>
+      </c>
       <c r="AB10">
         <v>24</v>
       </c>
@@ -1489,17 +1583,26 @@
       <c r="AD10">
         <v>14.3</v>
       </c>
+      <c r="AE10">
+        <v>25.9</v>
+      </c>
       <c r="AF10">
         <v>9.6999999999999993</v>
       </c>
       <c r="AG10">
         <v>10.9</v>
       </c>
+      <c r="AH10">
+        <v>15.9</v>
+      </c>
       <c r="AI10">
         <v>9.1</v>
       </c>
+      <c r="AJ10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1528,10 +1631,13 @@
         <v>6.6</v>
       </c>
       <c r="J11">
-        <v>9.1999999999999993</v>
+        <v>11</v>
       </c>
       <c r="K11">
         <v>0</v>
+      </c>
+      <c r="L11">
+        <v>6.6</v>
       </c>
       <c r="M11">
         <v>9.6</v>
@@ -1540,14 +1646,20 @@
         <v>7.9</v>
       </c>
       <c r="O11">
-        <v>10.3</v>
+        <v>11.7</v>
       </c>
       <c r="P11">
         <v>1.4</v>
       </c>
+      <c r="Q11">
+        <v>12</v>
+      </c>
       <c r="R11">
         <v>11.4</v>
       </c>
+      <c r="S11">
+        <v>13.7</v>
+      </c>
       <c r="T11">
         <v>6.8</v>
       </c>
@@ -1557,11 +1669,14 @@
       <c r="V11">
         <v>9.6</v>
       </c>
+      <c r="W11">
+        <v>14.6</v>
+      </c>
       <c r="X11">
         <v>7.4</v>
       </c>
       <c r="Y11">
-        <v>13</v>
+        <v>13.4</v>
       </c>
       <c r="Z11">
         <v>12</v>
@@ -1570,22 +1685,22 @@
         <v>19</v>
       </c>
       <c r="AB11">
-        <v>25</v>
+        <v>29.9</v>
       </c>
       <c r="AC11">
-        <v>16</v>
+        <v>15.7</v>
       </c>
       <c r="AD11">
         <v>13</v>
       </c>
       <c r="AE11">
-        <v>23</v>
+        <v>22.6</v>
       </c>
       <c r="AF11">
-        <v>11</v>
+        <v>11.2</v>
       </c>
       <c r="AG11">
-        <v>14</v>
+        <v>14.2</v>
       </c>
       <c r="AH11">
         <v>8</v>
@@ -1597,7 +1712,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1607,6 +1722,9 @@
       <c r="C12">
         <v>5.2</v>
       </c>
+      <c r="D12">
+        <v>2.7</v>
+      </c>
       <c r="E12">
         <v>6.9</v>
       </c>
@@ -1622,8 +1740,20 @@
       <c r="I12">
         <v>4.3</v>
       </c>
+      <c r="J12">
+        <v>8.5</v>
+      </c>
+      <c r="K12">
+        <v>6.6</v>
+      </c>
       <c r="L12">
         <v>0</v>
+      </c>
+      <c r="M12">
+        <v>13</v>
+      </c>
+      <c r="N12">
+        <v>5.9</v>
       </c>
       <c r="O12">
         <v>8.1999999999999993</v>
@@ -1631,12 +1761,24 @@
       <c r="P12">
         <v>4.3</v>
       </c>
+      <c r="Q12">
+        <v>12.8</v>
+      </c>
+      <c r="R12">
+        <v>18.2</v>
+      </c>
+      <c r="S12">
+        <v>11.3</v>
+      </c>
       <c r="T12">
         <v>3.5</v>
       </c>
       <c r="U12">
         <v>5.7</v>
       </c>
+      <c r="V12">
+        <v>6.9</v>
+      </c>
       <c r="W12">
         <v>12.5</v>
       </c>
@@ -1646,12 +1788,24 @@
       <c r="Y12">
         <v>11</v>
       </c>
+      <c r="Z12">
+        <v>22</v>
+      </c>
       <c r="AA12">
         <v>16.399999999999999</v>
       </c>
+      <c r="AB12">
+        <v>31.3</v>
+      </c>
+      <c r="AC12">
+        <v>16</v>
+      </c>
       <c r="AD12">
         <v>10.3</v>
       </c>
+      <c r="AE12">
+        <v>28.4</v>
+      </c>
       <c r="AF12">
         <v>8</v>
       </c>
@@ -1668,7 +1822,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1678,6 +1832,9 @@
       <c r="C13">
         <v>5.9</v>
       </c>
+      <c r="D13">
+        <v>12.9</v>
+      </c>
       <c r="E13">
         <v>6.7</v>
       </c>
@@ -1690,11 +1847,26 @@
       <c r="H13">
         <v>3.7</v>
       </c>
+      <c r="I13">
+        <v>11.8</v>
+      </c>
+      <c r="J13">
+        <v>10.8</v>
+      </c>
       <c r="K13">
         <v>9.6</v>
       </c>
+      <c r="L13">
+        <v>13</v>
+      </c>
       <c r="M13">
         <v>0</v>
+      </c>
+      <c r="N13">
+        <v>13.4</v>
+      </c>
+      <c r="O13">
+        <v>12.7</v>
       </c>
       <c r="P13">
         <v>10.4</v>
@@ -1705,23 +1877,62 @@
       <c r="R13">
         <v>1.9</v>
       </c>
+      <c r="S13">
+        <v>13.2</v>
+      </c>
+      <c r="T13">
+        <v>15.1</v>
+      </c>
+      <c r="U13">
+        <v>16</v>
+      </c>
+      <c r="V13">
+        <v>16.100000000000001</v>
+      </c>
       <c r="W13">
         <v>9.6</v>
       </c>
       <c r="X13">
         <v>15.1</v>
       </c>
+      <c r="Y13">
+        <v>29.1</v>
+      </c>
+      <c r="Z13">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="AA13">
+        <v>30.8</v>
+      </c>
       <c r="AB13">
         <v>15.8</v>
       </c>
       <c r="AC13">
         <v>10.3</v>
       </c>
+      <c r="AD13">
+        <v>22.8</v>
+      </c>
       <c r="AE13">
         <v>14.7</v>
       </c>
+      <c r="AF13">
+        <v>20</v>
+      </c>
+      <c r="AG13">
+        <v>23.8</v>
+      </c>
+      <c r="AH13">
+        <v>21.5</v>
+      </c>
+      <c r="AI13">
+        <v>18.3</v>
+      </c>
+      <c r="AJ13">
+        <v>41.3</v>
+      </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1731,6 +1942,9 @@
       <c r="C14">
         <v>6.4</v>
       </c>
+      <c r="D14">
+        <v>4.5999999999999996</v>
+      </c>
       <c r="E14">
         <v>5.0999999999999996</v>
       </c>
@@ -1746,9 +1960,18 @@
       <c r="I14">
         <v>1.8</v>
       </c>
+      <c r="J14">
+        <v>1.9</v>
+      </c>
       <c r="K14">
         <v>7.9</v>
       </c>
+      <c r="L14">
+        <v>5.9</v>
+      </c>
+      <c r="M14">
+        <v>13.4</v>
+      </c>
       <c r="N14">
         <v>0</v>
       </c>
@@ -1764,12 +1987,18 @@
       <c r="R14">
         <v>12.6</v>
       </c>
+      <c r="S14">
+        <v>7.2</v>
+      </c>
       <c r="T14">
         <v>4</v>
       </c>
       <c r="U14">
         <v>2.6</v>
       </c>
+      <c r="V14">
+        <v>2.9</v>
+      </c>
       <c r="W14">
         <v>8.8000000000000007</v>
       </c>
@@ -1779,15 +2008,24 @@
       <c r="Y14">
         <v>12.2</v>
       </c>
+      <c r="Z14">
+        <v>22.4</v>
+      </c>
       <c r="AA14">
         <v>16.5</v>
       </c>
+      <c r="AB14">
+        <v>30.7</v>
+      </c>
       <c r="AC14">
         <v>11.4</v>
       </c>
       <c r="AD14">
         <v>10.6</v>
       </c>
+      <c r="AE14">
+        <v>28.7</v>
+      </c>
       <c r="AF14">
         <v>6.1</v>
       </c>
@@ -1804,7 +2042,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1823,6 +2061,9 @@
       <c r="F15">
         <v>9.3000000000000007</v>
       </c>
+      <c r="G15">
+        <v>3.4</v>
+      </c>
       <c r="H15">
         <v>6.9</v>
       </c>
@@ -1832,20 +2073,29 @@
       <c r="J15">
         <v>1.6</v>
       </c>
+      <c r="K15">
+        <v>11.7</v>
+      </c>
       <c r="L15">
         <v>8.1999999999999993</v>
       </c>
+      <c r="M15">
+        <v>12.7</v>
+      </c>
       <c r="N15">
         <v>3.6</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
+      <c r="P15">
+        <v>11.7</v>
+      </c>
       <c r="Q15">
         <v>6</v>
       </c>
       <c r="R15">
-        <v>11</v>
+        <v>11.1</v>
       </c>
       <c r="S15">
         <v>1.9</v>
@@ -1863,40 +2113,46 @@
         <v>5.3</v>
       </c>
       <c r="X15">
-        <v>18</v>
+        <v>23.1</v>
       </c>
       <c r="Y15">
-        <v>16</v>
+        <v>15.6</v>
       </c>
       <c r="Z15">
         <v>15</v>
       </c>
       <c r="AA15">
-        <v>20</v>
+        <v>19.5</v>
       </c>
       <c r="AB15">
-        <v>25</v>
+        <v>26.9</v>
       </c>
       <c r="AC15">
-        <v>8</v>
+        <v>7.9</v>
       </c>
       <c r="AD15">
-        <v>14</v>
+        <v>13.8</v>
       </c>
       <c r="AE15">
-        <v>25</v>
+        <v>27.9</v>
       </c>
       <c r="AF15">
         <v>9</v>
       </c>
       <c r="AG15">
-        <v>10</v>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="AH15">
+        <v>17.899999999999999</v>
       </c>
       <c r="AI15">
         <v>8.1</v>
       </c>
+      <c r="AJ15">
+        <v>29.4</v>
+      </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1945,8 +2201,14 @@
       <c r="P16">
         <v>0</v>
       </c>
+      <c r="Q16">
+        <v>14.2</v>
+      </c>
       <c r="R16">
-        <v>12.2</v>
+        <v>12.3</v>
+      </c>
+      <c r="S16">
+        <v>15.9</v>
       </c>
       <c r="T16">
         <v>7.7</v>
@@ -1957,35 +2219,38 @@
       <c r="V16">
         <v>10.8</v>
       </c>
+      <c r="W16">
+        <v>16.8</v>
+      </c>
       <c r="X16">
         <v>6</v>
       </c>
       <c r="Y16">
-        <v>14</v>
+        <v>13.5</v>
       </c>
       <c r="Z16">
         <v>13</v>
       </c>
       <c r="AA16">
-        <v>19</v>
+        <v>19.2</v>
       </c>
       <c r="AB16">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="AC16">
-        <v>17</v>
+        <v>17.8</v>
       </c>
       <c r="AD16">
-        <v>13</v>
+        <v>13.4</v>
       </c>
       <c r="AE16">
-        <v>23</v>
+        <v>22.8</v>
       </c>
       <c r="AF16">
-        <v>12</v>
+        <v>12.1</v>
       </c>
       <c r="AG16">
-        <v>15</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="AH16">
         <v>7.1</v>
@@ -1997,7 +2262,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2028,6 +2293,12 @@
       <c r="J17">
         <v>5.2</v>
       </c>
+      <c r="K17">
+        <v>12</v>
+      </c>
+      <c r="L17">
+        <v>12.8</v>
+      </c>
       <c r="M17">
         <v>7.2</v>
       </c>
@@ -2037,6 +2308,9 @@
       <c r="O17">
         <v>6</v>
       </c>
+      <c r="P17">
+        <v>14.2</v>
+      </c>
       <c r="Q17">
         <v>0</v>
       </c>
@@ -2046,6 +2320,12 @@
       <c r="S17">
         <v>5.0999999999999996</v>
       </c>
+      <c r="T17">
+        <v>14.7</v>
+      </c>
+      <c r="U17">
+        <v>14.1</v>
+      </c>
       <c r="V17">
         <v>11.1</v>
       </c>
@@ -2053,37 +2333,46 @@
         <v>2.5</v>
       </c>
       <c r="X17">
-        <v>19</v>
+        <v>24.1</v>
       </c>
       <c r="Y17">
-        <v>21</v>
+        <v>27.9</v>
       </c>
       <c r="Z17">
         <v>11</v>
       </c>
       <c r="AA17">
-        <v>25</v>
+        <v>29.1</v>
       </c>
       <c r="AB17">
-        <v>20</v>
+        <v>19.7</v>
       </c>
       <c r="AC17">
         <v>3.6</v>
       </c>
       <c r="AD17">
-        <v>19</v>
+        <v>20.9</v>
       </c>
       <c r="AE17">
-        <v>20</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="AF17">
-        <v>15</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="AG17">
-        <v>16</v>
+        <v>21.1</v>
+      </c>
+      <c r="AH17">
+        <v>21.4</v>
+      </c>
+      <c r="AI17">
+        <v>15.6</v>
+      </c>
+      <c r="AJ17">
+        <v>39.9</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2117,6 +2406,9 @@
       <c r="K18">
         <v>11.4</v>
       </c>
+      <c r="L18">
+        <v>18.2</v>
+      </c>
       <c r="M18">
         <v>1.9</v>
       </c>
@@ -2138,6 +2430,15 @@
       <c r="S18">
         <v>11.1</v>
       </c>
+      <c r="T18">
+        <v>15</v>
+      </c>
+      <c r="U18">
+        <v>15</v>
+      </c>
+      <c r="V18">
+        <v>21.3</v>
+      </c>
       <c r="W18">
         <v>9.1999999999999993</v>
       </c>
@@ -2154,13 +2455,13 @@
         <v>29</v>
       </c>
       <c r="AB18">
-        <v>15</v>
+        <v>14.6</v>
       </c>
       <c r="AC18">
-        <v>9</v>
+        <v>9.4</v>
       </c>
       <c r="AD18">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="AE18">
         <v>14</v>
@@ -2181,7 +2482,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2191,9 +2492,15 @@
       <c r="C19">
         <v>8.3000000000000007</v>
       </c>
+      <c r="D19">
+        <v>9.9</v>
+      </c>
       <c r="E19">
         <v>5</v>
       </c>
+      <c r="F19">
+        <v>20.2</v>
+      </c>
       <c r="G19">
         <v>4.8</v>
       </c>
@@ -2203,9 +2510,27 @@
       <c r="I19">
         <v>5.7</v>
       </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>13.7</v>
+      </c>
+      <c r="L19">
+        <v>11.3</v>
+      </c>
+      <c r="M19">
+        <v>13.2</v>
+      </c>
+      <c r="N19">
+        <v>7.2</v>
+      </c>
       <c r="O19">
         <v>1.9</v>
       </c>
+      <c r="P19">
+        <v>15.9</v>
+      </c>
       <c r="Q19">
         <v>5.0999999999999996</v>
       </c>
@@ -2221,23 +2546,53 @@
       <c r="U19">
         <v>7.4</v>
       </c>
+      <c r="V19">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="W19">
         <v>3.9</v>
       </c>
+      <c r="X19">
+        <v>25.4</v>
+      </c>
+      <c r="Y19">
+        <v>24.4</v>
+      </c>
+      <c r="Z19">
+        <v>21.3</v>
+      </c>
+      <c r="AA19">
+        <v>25.6</v>
+      </c>
+      <c r="AB19">
+        <v>23.8</v>
+      </c>
       <c r="AC19">
         <v>6.4</v>
       </c>
+      <c r="AD19">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="AE19">
+        <v>26.6</v>
+      </c>
       <c r="AF19">
         <v>10.4</v>
       </c>
       <c r="AG19">
         <v>10.9</v>
       </c>
+      <c r="AH19">
+        <v>20.7</v>
+      </c>
       <c r="AI19">
         <v>9.4</v>
       </c>
+      <c r="AJ19">
+        <v>32.6</v>
+      </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2259,6 +2614,9 @@
       <c r="G20">
         <v>6.5</v>
       </c>
+      <c r="H20">
+        <v>27.7</v>
+      </c>
       <c r="I20">
         <v>4.4000000000000004</v>
       </c>
@@ -2271,6 +2629,9 @@
       <c r="L20">
         <v>3.5</v>
       </c>
+      <c r="M20">
+        <v>15.1</v>
+      </c>
       <c r="N20">
         <v>4</v>
       </c>
@@ -2280,6 +2641,9 @@
       <c r="P20">
         <v>7.7</v>
       </c>
+      <c r="Q20">
+        <v>14.7</v>
+      </c>
       <c r="R20">
         <v>15</v>
       </c>
@@ -2295,8 +2659,11 @@
       <c r="V20">
         <v>3.7</v>
       </c>
+      <c r="W20">
+        <v>13.9</v>
+      </c>
       <c r="X20">
-        <v>13</v>
+        <v>12.5</v>
       </c>
       <c r="Y20">
         <v>8.6</v>
@@ -2305,25 +2672,25 @@
         <v>18</v>
       </c>
       <c r="AA20">
-        <v>14</v>
+        <v>13.5</v>
       </c>
       <c r="AB20">
-        <v>30</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="AC20">
-        <v>15</v>
+        <v>17.2</v>
       </c>
       <c r="AD20">
-        <v>7</v>
+        <v>7.3</v>
       </c>
       <c r="AE20">
-        <v>28</v>
+        <v>30.4</v>
       </c>
       <c r="AF20">
-        <v>4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AG20">
-        <v>7</v>
+        <v>7.4</v>
       </c>
       <c r="AH20">
         <v>9.5</v>
@@ -2335,7 +2702,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2357,6 +2724,9 @@
       <c r="G21">
         <v>6</v>
       </c>
+      <c r="H21">
+        <v>22</v>
+      </c>
       <c r="I21">
         <v>4.0999999999999996</v>
       </c>
@@ -2369,6 +2739,9 @@
       <c r="L21">
         <v>5.7</v>
       </c>
+      <c r="M21">
+        <v>16</v>
+      </c>
       <c r="N21">
         <v>2.6</v>
       </c>
@@ -2378,6 +2751,9 @@
       <c r="P21">
         <v>10</v>
       </c>
+      <c r="Q21">
+        <v>14.1</v>
+      </c>
       <c r="R21">
         <v>15</v>
       </c>
@@ -2393,8 +2769,11 @@
       <c r="V21">
         <v>0.9</v>
       </c>
+      <c r="W21">
+        <v>11.1</v>
+      </c>
       <c r="X21">
-        <v>15</v>
+        <v>15.2</v>
       </c>
       <c r="Y21">
         <v>9.8000000000000007</v>
@@ -2403,25 +2782,25 @@
         <v>18</v>
       </c>
       <c r="AA21">
-        <v>14</v>
+        <v>13.9</v>
       </c>
       <c r="AB21">
-        <v>30</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="AC21">
-        <v>14</v>
+        <v>13.7</v>
       </c>
       <c r="AD21">
         <v>8</v>
       </c>
       <c r="AE21">
-        <v>29</v>
+        <v>31.3</v>
       </c>
       <c r="AF21">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AG21">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="AH21">
         <v>12.2</v>
@@ -2433,7 +2812,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2443,6 +2822,9 @@
       <c r="C22">
         <v>8.9</v>
       </c>
+      <c r="D22">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="E22">
         <v>7.7</v>
       </c>
@@ -2452,12 +2834,27 @@
       <c r="G22">
         <v>6</v>
       </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
       <c r="I22">
         <v>4.3</v>
       </c>
+      <c r="J22">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="K22">
         <v>9.6</v>
       </c>
+      <c r="L22">
+        <v>6.9</v>
+      </c>
+      <c r="M22">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="N22">
+        <v>2.9</v>
+      </c>
       <c r="O22">
         <v>5.3</v>
       </c>
@@ -2467,6 +2864,12 @@
       <c r="Q22">
         <v>11.1</v>
       </c>
+      <c r="R22">
+        <v>21.3</v>
+      </c>
+      <c r="S22">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="T22">
         <v>3.7</v>
       </c>
@@ -2485,15 +2888,24 @@
       <c r="Y22">
         <v>10.4</v>
       </c>
+      <c r="Z22">
+        <v>25.1</v>
+      </c>
       <c r="AA22">
         <v>14.3</v>
       </c>
+      <c r="AB22">
+        <v>33.299999999999997</v>
+      </c>
       <c r="AC22">
         <v>13.2</v>
       </c>
       <c r="AD22">
         <v>8.5</v>
       </c>
+      <c r="AE22">
+        <v>31.4</v>
+      </c>
       <c r="AF22">
         <v>3.7</v>
       </c>
@@ -2510,7 +2922,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2541,6 +2953,9 @@
       <c r="J23">
         <v>5.2</v>
       </c>
+      <c r="K23">
+        <v>14.6</v>
+      </c>
       <c r="L23">
         <v>12.5</v>
       </c>
@@ -2553,6 +2968,9 @@
       <c r="O23">
         <v>5.3</v>
       </c>
+      <c r="P23">
+        <v>16.8</v>
+      </c>
       <c r="Q23">
         <v>2.5</v>
       </c>
@@ -2562,6 +2980,9 @@
       <c r="S23">
         <v>3.9</v>
       </c>
+      <c r="T23">
+        <v>13.9</v>
+      </c>
       <c r="U23">
         <v>11.1</v>
       </c>
@@ -2572,37 +2993,46 @@
         <v>0</v>
       </c>
       <c r="X23">
-        <v>21</v>
+        <v>26.7</v>
       </c>
       <c r="Y23">
-        <v>21</v>
+        <v>26.3</v>
       </c>
       <c r="Z23">
         <v>14</v>
       </c>
       <c r="AA23">
-        <v>25</v>
+        <v>27.5</v>
       </c>
       <c r="AB23">
-        <v>22</v>
+        <v>21.8</v>
       </c>
       <c r="AC23">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="AD23">
-        <v>19</v>
+        <v>19.3</v>
       </c>
       <c r="AE23">
-        <v>22</v>
+        <v>22.4</v>
       </c>
       <c r="AF23">
-        <v>14</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="AG23">
-        <v>15</v>
+        <v>14.7</v>
+      </c>
+      <c r="AH23">
+        <v>22.6</v>
+      </c>
+      <c r="AI23">
+        <v>13.8</v>
+      </c>
+      <c r="AJ23">
+        <v>34.6</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2630,6 +3060,9 @@
       <c r="I24">
         <v>13.8</v>
       </c>
+      <c r="J24">
+        <v>22.5</v>
+      </c>
       <c r="K24">
         <v>7.4</v>
       </c>
@@ -2642,12 +3075,21 @@
       <c r="N24">
         <v>15</v>
       </c>
+      <c r="O24">
+        <v>23.1</v>
+      </c>
       <c r="P24">
         <v>6</v>
       </c>
+      <c r="Q24">
+        <v>24.1</v>
+      </c>
       <c r="R24">
         <v>17</v>
       </c>
+      <c r="S24">
+        <v>25.4</v>
+      </c>
       <c r="T24">
         <v>12.5</v>
       </c>
@@ -2657,6 +3099,9 @@
       <c r="V24">
         <v>16.100000000000001</v>
       </c>
+      <c r="W24">
+        <v>26.7</v>
+      </c>
       <c r="X24">
         <v>0</v>
       </c>
@@ -2697,16 +3142,22 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25">
         <v>16</v>
       </c>
+      <c r="C25">
+        <v>30.7</v>
+      </c>
       <c r="D25">
         <v>14.4</v>
       </c>
+      <c r="E25">
+        <v>27.2</v>
+      </c>
       <c r="F25">
         <v>16</v>
       </c>
@@ -2719,12 +3170,18 @@
       <c r="I25">
         <v>13</v>
       </c>
+      <c r="J25">
+        <v>22.5</v>
+      </c>
       <c r="K25">
         <v>13.4</v>
       </c>
       <c r="L25">
         <v>11</v>
       </c>
+      <c r="M25">
+        <v>29.1</v>
+      </c>
       <c r="N25">
         <v>12.2</v>
       </c>
@@ -2734,9 +3191,15 @@
       <c r="P25">
         <v>13.5</v>
       </c>
+      <c r="Q25">
+        <v>27.9</v>
+      </c>
       <c r="R25">
         <v>23</v>
       </c>
+      <c r="S25">
+        <v>24.4</v>
+      </c>
       <c r="T25">
         <v>8.6</v>
       </c>
@@ -2746,6 +3209,9 @@
       <c r="V25">
         <v>10.4</v>
       </c>
+      <c r="W25">
+        <v>26.3</v>
+      </c>
       <c r="X25">
         <v>15.4</v>
       </c>
@@ -2786,7 +3252,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2796,6 +3262,9 @@
       <c r="C26">
         <v>10</v>
       </c>
+      <c r="D26">
+        <v>22.9</v>
+      </c>
       <c r="E26">
         <v>11</v>
       </c>
@@ -2811,9 +3280,21 @@
       <c r="I26">
         <v>14</v>
       </c>
+      <c r="J26">
+        <v>19.8</v>
+      </c>
       <c r="K26">
         <v>12</v>
       </c>
+      <c r="L26">
+        <v>22</v>
+      </c>
+      <c r="M26">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="N26">
+        <v>22.4</v>
+      </c>
       <c r="O26">
         <v>15</v>
       </c>
@@ -2826,12 +3307,18 @@
       <c r="R26">
         <v>4</v>
       </c>
+      <c r="S26">
+        <v>21.3</v>
+      </c>
       <c r="T26">
         <v>18</v>
       </c>
       <c r="U26">
         <v>18</v>
       </c>
+      <c r="V26">
+        <v>25.1</v>
+      </c>
       <c r="W26">
         <v>14</v>
       </c>
@@ -2875,16 +3362,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27">
         <v>21</v>
       </c>
+      <c r="C27">
+        <v>32</v>
+      </c>
       <c r="D27">
         <v>19.3</v>
       </c>
+      <c r="E27">
+        <v>28.6</v>
+      </c>
       <c r="F27">
         <v>22</v>
       </c>
@@ -2897,12 +3390,18 @@
       <c r="I27">
         <v>17.7</v>
       </c>
+      <c r="J27">
+        <v>23.7</v>
+      </c>
       <c r="K27">
         <v>19</v>
       </c>
       <c r="L27">
         <v>16.399999999999999</v>
       </c>
+      <c r="M27">
+        <v>30.8</v>
+      </c>
       <c r="N27">
         <v>16.5</v>
       </c>
@@ -2912,9 +3411,15 @@
       <c r="P27">
         <v>19.2</v>
       </c>
+      <c r="Q27">
+        <v>29.1</v>
+      </c>
       <c r="R27">
         <v>29</v>
       </c>
+      <c r="S27">
+        <v>25.6</v>
+      </c>
       <c r="T27">
         <v>13.5</v>
       </c>
@@ -2924,6 +3429,9 @@
       <c r="V27">
         <v>14.3</v>
       </c>
+      <c r="W27">
+        <v>27.5</v>
+      </c>
       <c r="X27">
         <v>21</v>
       </c>
@@ -2964,7 +3472,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2989,18 +3497,48 @@
       <c r="H28">
         <v>19.100000000000001</v>
       </c>
+      <c r="I28">
+        <v>36.9</v>
+      </c>
       <c r="J28">
         <v>24</v>
       </c>
+      <c r="K28">
+        <v>29.9</v>
+      </c>
+      <c r="L28">
+        <v>31.3</v>
+      </c>
       <c r="M28">
         <v>15.8</v>
       </c>
+      <c r="N28">
+        <v>30.7</v>
+      </c>
+      <c r="O28">
+        <v>26.9</v>
+      </c>
+      <c r="P28">
+        <v>32</v>
+      </c>
       <c r="Q28">
         <v>19.7</v>
       </c>
       <c r="R28">
         <v>14.6</v>
       </c>
+      <c r="S28">
+        <v>23.8</v>
+      </c>
+      <c r="T28">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="U28">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="V28">
+        <v>33.299999999999997</v>
+      </c>
       <c r="W28">
         <v>21.8</v>
       </c>
@@ -3044,7 +3582,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -3075,6 +3613,12 @@
       <c r="J29">
         <v>7.7</v>
       </c>
+      <c r="K29">
+        <v>15.7</v>
+      </c>
+      <c r="L29">
+        <v>16</v>
+      </c>
       <c r="M29">
         <v>10.3</v>
       </c>
@@ -3084,6 +3628,9 @@
       <c r="O29">
         <v>7.9</v>
       </c>
+      <c r="P29">
+        <v>17.8</v>
+      </c>
       <c r="Q29">
         <v>3.6</v>
       </c>
@@ -3093,6 +3640,9 @@
       <c r="S29">
         <v>6.4</v>
       </c>
+      <c r="T29">
+        <v>17.2</v>
+      </c>
       <c r="U29">
         <v>13.7</v>
       </c>
@@ -3142,7 +3692,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -3155,6 +3705,9 @@
       <c r="D30">
         <v>13.2</v>
       </c>
+      <c r="E30">
+        <v>19.899999999999999</v>
+      </c>
       <c r="F30">
         <v>16</v>
       </c>
@@ -3176,6 +3729,9 @@
       <c r="L30">
         <v>10.3</v>
       </c>
+      <c r="M30">
+        <v>22.8</v>
+      </c>
       <c r="N30">
         <v>10.6</v>
       </c>
@@ -3185,6 +3741,15 @@
       <c r="P30">
         <v>13.4</v>
       </c>
+      <c r="Q30">
+        <v>20.9</v>
+      </c>
+      <c r="R30">
+        <v>28</v>
+      </c>
+      <c r="S30">
+        <v>17.399999999999999</v>
+      </c>
       <c r="T30">
         <v>7.3</v>
       </c>
@@ -3194,6 +3759,9 @@
       <c r="V30">
         <v>8.5</v>
       </c>
+      <c r="W30">
+        <v>19.3</v>
+      </c>
       <c r="X30">
         <v>16</v>
       </c>
@@ -3234,7 +3802,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -3259,12 +3827,27 @@
       <c r="H31">
         <v>18.3</v>
       </c>
+      <c r="I31">
+        <v>29.5</v>
+      </c>
+      <c r="J31">
+        <v>25.9</v>
+      </c>
       <c r="K31">
         <v>22.6</v>
       </c>
+      <c r="L31">
+        <v>28.4</v>
+      </c>
       <c r="M31">
         <v>14.7</v>
       </c>
+      <c r="N31">
+        <v>28.7</v>
+      </c>
+      <c r="O31">
+        <v>27.9</v>
+      </c>
       <c r="P31">
         <v>22.8</v>
       </c>
@@ -3274,6 +3857,18 @@
       <c r="R31">
         <v>14</v>
       </c>
+      <c r="S31">
+        <v>26.6</v>
+      </c>
+      <c r="T31">
+        <v>30.4</v>
+      </c>
+      <c r="U31">
+        <v>31.3</v>
+      </c>
+      <c r="V31">
+        <v>31.4</v>
+      </c>
       <c r="W31">
         <v>22.4</v>
       </c>
@@ -3317,7 +3912,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -3354,6 +3949,9 @@
       <c r="L32">
         <v>8</v>
       </c>
+      <c r="M32">
+        <v>20</v>
+      </c>
       <c r="N32">
         <v>6.1</v>
       </c>
@@ -3363,6 +3961,9 @@
       <c r="P32">
         <v>12.1</v>
       </c>
+      <c r="Q32">
+        <v>18.100000000000001</v>
+      </c>
       <c r="R32">
         <v>19</v>
       </c>
@@ -3378,6 +3979,9 @@
       <c r="V32">
         <v>3.7</v>
       </c>
+      <c r="W32">
+        <v>16.600000000000001</v>
+      </c>
       <c r="X32">
         <v>16</v>
       </c>
@@ -3418,7 +4022,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -3455,12 +4059,21 @@
       <c r="L33">
         <v>10.9</v>
       </c>
+      <c r="M33">
+        <v>23.8</v>
+      </c>
       <c r="N33">
         <v>7.9</v>
       </c>
       <c r="O33">
         <v>9.8000000000000007</v>
       </c>
+      <c r="P33">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="Q33">
+        <v>21.1</v>
+      </c>
       <c r="R33">
         <v>20</v>
       </c>
@@ -3509,6 +4122,9 @@
       <c r="AG33">
         <v>0</v>
       </c>
+      <c r="AH33">
+        <v>27.3</v>
+      </c>
       <c r="AI33">
         <v>2.2000000000000002</v>
       </c>
@@ -3516,7 +4132,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -3544,21 +4160,36 @@
       <c r="I34">
         <v>12.5</v>
       </c>
+      <c r="J34">
+        <v>15.9</v>
+      </c>
       <c r="K34">
         <v>8</v>
       </c>
       <c r="L34">
         <v>8.3000000000000007</v>
       </c>
+      <c r="M34">
+        <v>21.5</v>
+      </c>
       <c r="N34">
         <v>13</v>
       </c>
+      <c r="O34">
+        <v>17.899999999999999</v>
+      </c>
       <c r="P34">
         <v>7.1</v>
       </c>
+      <c r="Q34">
+        <v>21.4</v>
+      </c>
       <c r="R34">
         <v>19</v>
       </c>
+      <c r="S34">
+        <v>20.7</v>
+      </c>
       <c r="T34">
         <v>9.5</v>
       </c>
@@ -3568,6 +4199,9 @@
       <c r="V34">
         <v>13.2</v>
       </c>
+      <c r="W34">
+        <v>22.6</v>
+      </c>
       <c r="X34">
         <v>5.9</v>
       </c>
@@ -3595,14 +4229,20 @@
       <c r="AF34">
         <v>12.3</v>
       </c>
+      <c r="AG34">
+        <v>27.3</v>
+      </c>
       <c r="AH34">
         <v>0</v>
+      </c>
+      <c r="AI34">
+        <v>14.5</v>
       </c>
       <c r="AJ34">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3639,6 +4279,9 @@
       <c r="L35">
         <v>8.6999999999999993</v>
       </c>
+      <c r="M35">
+        <v>18.3</v>
+      </c>
       <c r="N35">
         <v>5.8</v>
       </c>
@@ -3648,6 +4291,9 @@
       <c r="P35">
         <v>13</v>
       </c>
+      <c r="Q35">
+        <v>15.6</v>
+      </c>
       <c r="R35">
         <v>18</v>
       </c>
@@ -3663,6 +4309,9 @@
       <c r="V35">
         <v>3.2</v>
       </c>
+      <c r="W35">
+        <v>13.8</v>
+      </c>
       <c r="X35">
         <v>18</v>
       </c>
@@ -3693,6 +4342,9 @@
       <c r="AG35">
         <v>2.2000000000000002</v>
       </c>
+      <c r="AH35">
+        <v>14.5</v>
+      </c>
       <c r="AI35">
         <v>0</v>
       </c>
@@ -3700,34 +4352,64 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36">
         <v>28</v>
       </c>
+      <c r="C36">
+        <v>49.1</v>
+      </c>
+      <c r="D36">
+        <v>39.6</v>
+      </c>
+      <c r="E36">
+        <v>45.6</v>
+      </c>
       <c r="F36">
         <v>28</v>
       </c>
+      <c r="G36">
+        <v>43.4</v>
+      </c>
       <c r="H36">
         <v>31</v>
       </c>
+      <c r="I36">
+        <v>42</v>
+      </c>
+      <c r="J36">
+        <v>31</v>
+      </c>
       <c r="K36">
         <v>24.3</v>
       </c>
       <c r="L36">
         <v>22.5</v>
       </c>
+      <c r="M36">
+        <v>41.3</v>
+      </c>
       <c r="N36">
         <v>24</v>
       </c>
+      <c r="O36">
+        <v>29.4</v>
+      </c>
       <c r="P36">
         <v>24</v>
       </c>
+      <c r="Q36">
+        <v>39.9</v>
+      </c>
       <c r="R36">
         <v>35</v>
       </c>
+      <c r="S36">
+        <v>32.6</v>
+      </c>
       <c r="T36">
         <v>20.399999999999999</v>
       </c>
@@ -3737,6 +4419,9 @@
       <c r="V36">
         <v>22.1</v>
       </c>
+      <c r="W36">
+        <v>34.6</v>
+      </c>
       <c r="X36">
         <v>23.5</v>
       </c>
@@ -3769,6 +4454,9 @@
       </c>
       <c r="AH36">
         <v>17.899999999999999</v>
+      </c>
+      <c r="AI36">
+        <v>20.8</v>
       </c>
       <c r="AJ36">
         <v>0</v>
@@ -3784,12 +4472,12 @@
   <dimension ref="A1:AJ36"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AJ1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="1" customFormat="1">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3896,7 +4584,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4006,7 +4694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4116,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4226,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -4336,7 +5024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -4446,7 +5134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4556,7 +5244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4666,7 +5354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4776,7 +5464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4886,7 +5574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4996,7 +5684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -5106,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -5216,7 +5904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -5326,7 +6014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -5436,7 +6124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -5546,7 +6234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -5656,7 +6344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -5766,7 +6454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -5876,7 +6564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -5986,7 +6674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -6096,7 +6784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -6206,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -6316,7 +7004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -6426,7 +7114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -6536,7 +7224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -6646,7 +7334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -6756,7 +7444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -6866,7 +7554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -6976,7 +7664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -7086,7 +7774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -7196,7 +7884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -7306,7 +7994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -7416,7 +8104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -7526,7 +8214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -7636,7 +8324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36">
       <c r="A36" t="s">
         <v>34</v>
       </c>

</xml_diff>